<commit_message>
COBie to COBieLiteUK fixes and enhancements.
</commit_message>
<xml_diff>
--- a/Tests/TestFiles/2012-03-23-Duplex-Design.xlsx
+++ b/Tests/TestFiles/2012-03-23-Duplex-Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="252" yWindow="648" windowWidth="9756" windowHeight="9360" tabRatio="804" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="252" yWindow="648" windowWidth="9756" windowHeight="9360" tabRatio="804" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12801" uniqueCount="6702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12747" uniqueCount="6703">
   <si>
     <t>Title</t>
   </si>
@@ -20228,6 +20228,9 @@
   </si>
   <si>
     <t>The phase identification used for the device electrical input. This should be the same phase identifier that is used for the conductor segment providing the electrical service to the device. In general, it is recommended that IEC mmendations for phase identification are used (L1, L2 etc.). However, other phase identifiers may be used such as bycolor (Red, Blue, Yellow) or by number (1, 2, 3) etc.recommended that IEC recommendations for phase identification are used(L1, L2 etc.). However, other phase identifiers may be used such as bycolor (Red, Blue, Yellow) or by number (1, 2, 3) etc.</t>
+  </si>
+  <si>
+    <t>Shower Stall-1, Sink Type A-1, Sink Type B-1, Sink Type C-1, Sink Type C-2, Toilet-1, Toilet-2</t>
   </si>
 </sst>
 </file>
@@ -20864,7 +20867,7 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -21068,6 +21071,7 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="24" fillId="36" borderId="11" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -25887,7 +25891,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L14" sqref="L13:L14"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28099,7 +28103,7 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -68895,13 +68899,13 @@
   <sheetPr codeName="Sheet9">
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -68959,8 +68963,8 @@
       <c r="D2" s="55" t="s">
         <v>1235</v>
       </c>
-      <c r="E2" s="55" t="s">
-        <v>1001</v>
+      <c r="E2" s="94" t="s">
+        <v>6702</v>
       </c>
       <c r="F2" s="56" t="s">
         <v>250</v>
@@ -68977,7 +68981,7 @@
     </row>
     <row r="3" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="54" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="B3" s="55" t="s">
         <v>107</v>
@@ -68989,7 +68993,7 @@
         <v>1235</v>
       </c>
       <c r="E3" s="55" t="s">
-        <v>1081</v>
+        <v>1004</v>
       </c>
       <c r="F3" s="56" t="s">
         <v>250</v>
@@ -69006,7 +69010,7 @@
     </row>
     <row r="4" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="54" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="B4" s="55" t="s">
         <v>107</v>
@@ -69018,7 +69022,7 @@
         <v>1235</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="F4" s="56" t="s">
         <v>250</v>
@@ -69035,7 +69039,7 @@
     </row>
     <row r="5" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="54" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="B5" s="55" t="s">
         <v>107</v>
@@ -69047,7 +69051,7 @@
         <v>1235</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="F5" s="56" t="s">
         <v>250</v>
@@ -69064,7 +69068,7 @@
     </row>
     <row r="6" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="54" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="B6" s="55" t="s">
         <v>107</v>
@@ -69076,7 +69080,7 @@
         <v>1235</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>1096</v>
+        <v>1099</v>
       </c>
       <c r="F6" s="56" t="s">
         <v>250</v>
@@ -69093,7 +69097,7 @@
     </row>
     <row r="7" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="54" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="B7" s="55" t="s">
         <v>107</v>
@@ -69105,7 +69109,7 @@
         <v>1235</v>
       </c>
       <c r="E7" s="55" t="s">
-        <v>1153</v>
+        <v>1102</v>
       </c>
       <c r="F7" s="56" t="s">
         <v>250</v>
@@ -69122,7 +69126,7 @@
     </row>
     <row r="8" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="54" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="B8" s="55" t="s">
         <v>107</v>
@@ -69134,7 +69138,7 @@
         <v>1235</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>1156</v>
+        <v>1159</v>
       </c>
       <c r="F8" s="56" t="s">
         <v>250</v>
@@ -69163,7 +69167,7 @@
         <v>1235</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>1004</v>
+        <v>1162</v>
       </c>
       <c r="F9" s="56" t="s">
         <v>250</v>
@@ -69180,7 +69184,7 @@
     </row>
     <row r="10" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="54" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="B10" s="55" t="s">
         <v>107</v>
@@ -69189,10 +69193,10 @@
         <v>108</v>
       </c>
       <c r="D10" s="55" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>1084</v>
+        <v>459</v>
       </c>
       <c r="F10" s="56" t="s">
         <v>250</v>
@@ -69209,7 +69213,7 @@
     </row>
     <row r="11" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="54" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="B11" s="55" t="s">
         <v>107</v>
@@ -69218,10 +69222,10 @@
         <v>108</v>
       </c>
       <c r="D11" s="55" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>1090</v>
+        <v>956</v>
       </c>
       <c r="F11" s="56" t="s">
         <v>250</v>
@@ -69238,7 +69242,7 @@
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="54" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="B12" s="55" t="s">
         <v>107</v>
@@ -69247,10 +69251,10 @@
         <v>108</v>
       </c>
       <c r="D12" s="55" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>1099</v>
+        <v>974</v>
       </c>
       <c r="F12" s="56" t="s">
         <v>250</v>
@@ -69267,22 +69271,22 @@
     </row>
     <row r="13" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="54" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>108</v>
+        <v>1239</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>1102</v>
+        <v>983</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>250</v>
+        <v>1240</v>
       </c>
       <c r="G13" s="56" t="s">
         <v>251</v>
@@ -69296,7 +69300,7 @@
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="54" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="B14" s="55" t="s">
         <v>107</v>
@@ -69305,10 +69309,10 @@
         <v>108</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>1159</v>
+        <v>452</v>
       </c>
       <c r="F14" s="56" t="s">
         <v>250</v>
@@ -69325,7 +69329,7 @@
     </row>
     <row r="15" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="54" t="s">
-        <v>1236</v>
+        <v>1241</v>
       </c>
       <c r="B15" s="55" t="s">
         <v>107</v>
@@ -69334,18 +69338,18 @@
         <v>108</v>
       </c>
       <c r="D15" s="55" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>1162</v>
-      </c>
-      <c r="F15" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="F15" s="58" t="s">
         <v>250</v>
       </c>
-      <c r="G15" s="56" t="s">
+      <c r="G15" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="H15" s="56" t="s">
+      <c r="H15" s="58" t="s">
         <v>94</v>
       </c>
       <c r="I15" s="57" t="s">
@@ -69353,28 +69357,28 @@
       </c>
     </row>
     <row r="16" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="54" t="s">
-        <v>1237</v>
-      </c>
-      <c r="B16" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="55" t="s">
+      <c r="A16" s="59" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D16" s="60" t="s">
         <v>1238</v>
       </c>
-      <c r="E16" s="55" t="s">
-        <v>459</v>
-      </c>
-      <c r="F16" s="56" t="s">
-        <v>250</v>
-      </c>
-      <c r="G16" s="56" t="s">
+      <c r="E16" s="60" t="s">
+        <v>947</v>
+      </c>
+      <c r="F16" s="61" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G16" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="H16" s="56" t="s">
+      <c r="H16" s="61" t="s">
         <v>94</v>
       </c>
       <c r="I16" s="57" t="s">
@@ -69383,7 +69387,7 @@
     </row>
     <row r="17" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="54" t="s">
-        <v>1237</v>
+        <v>1241</v>
       </c>
       <c r="B17" s="55" t="s">
         <v>107</v>
@@ -69395,15 +69399,15 @@
         <v>1238</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>956</v>
-      </c>
-      <c r="F17" s="56" t="s">
-        <v>250</v>
-      </c>
-      <c r="G17" s="56" t="s">
+        <v>950</v>
+      </c>
+      <c r="F17" s="58" t="s">
+        <v>1244</v>
+      </c>
+      <c r="G17" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="H17" s="56" t="s">
+      <c r="H17" s="58" t="s">
         <v>94</v>
       </c>
       <c r="I17" s="57" t="s">
@@ -69412,7 +69416,7 @@
     </row>
     <row r="18" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="54" t="s">
-        <v>1237</v>
+        <v>1241</v>
       </c>
       <c r="B18" s="55" t="s">
         <v>107</v>
@@ -69424,15 +69428,15 @@
         <v>1238</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>974</v>
-      </c>
-      <c r="F18" s="56" t="s">
+        <v>953</v>
+      </c>
+      <c r="F18" s="58" t="s">
         <v>250</v>
       </c>
-      <c r="G18" s="56" t="s">
+      <c r="G18" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="H18" s="56" t="s">
+      <c r="H18" s="58" t="s">
         <v>94</v>
       </c>
       <c r="I18" s="57" t="s">
@@ -69441,27 +69445,27 @@
     </row>
     <row r="19" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="54" t="s">
-        <v>1237</v>
+        <v>1241</v>
       </c>
       <c r="B19" s="55" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>1239</v>
+        <v>108</v>
       </c>
       <c r="D19" s="55" t="s">
         <v>1238</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>983</v>
-      </c>
-      <c r="F19" s="56" t="s">
-        <v>1240</v>
-      </c>
-      <c r="G19" s="56" t="s">
+        <v>959</v>
+      </c>
+      <c r="F19" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G19" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="H19" s="56" t="s">
+      <c r="H19" s="58" t="s">
         <v>94</v>
       </c>
       <c r="I19" s="57" t="s">
@@ -69470,27 +69474,27 @@
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="54" t="s">
-        <v>1234</v>
+        <v>1241</v>
       </c>
       <c r="B20" s="55" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>108</v>
+        <v>1245</v>
       </c>
       <c r="D20" s="55" t="s">
         <v>1238</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>452</v>
-      </c>
-      <c r="F20" s="56" t="s">
-        <v>250</v>
-      </c>
-      <c r="G20" s="56" t="s">
+        <v>962</v>
+      </c>
+      <c r="F20" s="58" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G20" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="H20" s="56" t="s">
+      <c r="H20" s="58" t="s">
         <v>94</v>
       </c>
       <c r="I20" s="57" t="s">
@@ -69498,28 +69502,28 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="59" t="s">
         <v>1241</v>
       </c>
-      <c r="B21" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="55" t="s">
+      <c r="B21" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="59" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D21" s="60" t="s">
         <v>1238</v>
       </c>
-      <c r="E21" s="55" t="s">
-        <v>463</v>
-      </c>
-      <c r="F21" s="58" t="s">
-        <v>250</v>
-      </c>
-      <c r="G21" s="58" t="s">
+      <c r="E21" s="60" t="s">
+        <v>965</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>1248</v>
+      </c>
+      <c r="G21" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="H21" s="58" t="s">
+      <c r="H21" s="61" t="s">
         <v>94</v>
       </c>
       <c r="I21" s="57" t="s">
@@ -69527,28 +69531,28 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="54" t="s">
         <v>1241</v>
       </c>
-      <c r="B22" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" s="59" t="s">
-        <v>1242</v>
-      </c>
-      <c r="D22" s="60" t="s">
+      <c r="B22" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="55" t="s">
         <v>1238</v>
       </c>
-      <c r="E22" s="60" t="s">
-        <v>947</v>
-      </c>
-      <c r="F22" s="61" t="s">
-        <v>1243</v>
-      </c>
-      <c r="G22" s="61" t="s">
+      <c r="E22" s="55" t="s">
+        <v>968</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G22" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="H22" s="61" t="s">
+      <c r="H22" s="58" t="s">
         <v>94</v>
       </c>
       <c r="I22" s="57" t="s">
@@ -69556,28 +69560,28 @@
       </c>
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="59" t="s">
         <v>1241</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="55" t="s">
+      <c r="D23" s="60" t="s">
         <v>1238</v>
       </c>
-      <c r="E23" s="55" t="s">
-        <v>950</v>
-      </c>
-      <c r="F23" s="58" t="s">
-        <v>1244</v>
-      </c>
-      <c r="G23" s="58" t="s">
+      <c r="E23" s="60" t="s">
+        <v>971</v>
+      </c>
+      <c r="F23" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="G23" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="H23" s="58" t="s">
+      <c r="H23" s="61" t="s">
         <v>94</v>
       </c>
       <c r="I23" s="57" t="s">
@@ -69598,7 +69602,7 @@
         <v>1238</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>953</v>
+        <v>977</v>
       </c>
       <c r="F24" s="58" t="s">
         <v>250</v>
@@ -69627,7 +69631,7 @@
         <v>1238</v>
       </c>
       <c r="E25" s="55" t="s">
-        <v>959</v>
+        <v>980</v>
       </c>
       <c r="F25" s="58" t="s">
         <v>250</v>
@@ -69650,16 +69654,16 @@
         <v>91</v>
       </c>
       <c r="C26" s="54" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="D26" s="55" t="s">
         <v>1238</v>
       </c>
       <c r="E26" s="55" t="s">
-        <v>962</v>
+        <v>986</v>
       </c>
       <c r="F26" s="58" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="G26" s="58" t="s">
         <v>251</v>
@@ -69672,28 +69676,28 @@
       </c>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="59" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B27" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="59" t="s">
-        <v>1247</v>
-      </c>
-      <c r="D27" s="60" t="s">
+      <c r="A27" s="54" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="55" t="s">
         <v>1238</v>
       </c>
-      <c r="E27" s="60" t="s">
-        <v>965</v>
-      </c>
-      <c r="F27" s="61" t="s">
-        <v>1248</v>
-      </c>
-      <c r="G27" s="61" t="s">
+      <c r="E27" s="55" t="s">
+        <v>456</v>
+      </c>
+      <c r="F27" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G27" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="H27" s="61" t="s">
+      <c r="H27" s="58" t="s">
         <v>94</v>
       </c>
       <c r="I27" s="57" t="s">
@@ -69702,7 +69706,7 @@
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="54" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="B28" s="55" t="s">
         <v>107</v>
@@ -69711,18 +69715,18 @@
         <v>108</v>
       </c>
       <c r="D28" s="55" t="s">
-        <v>1238</v>
+        <v>1249</v>
       </c>
       <c r="E28" s="55" t="s">
-        <v>968</v>
-      </c>
-      <c r="F28" s="58" t="s">
+        <v>855</v>
+      </c>
+      <c r="F28" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="G28" s="58" t="s">
+      <c r="G28" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="H28" s="58" t="s">
+      <c r="H28" s="56" t="s">
         <v>94</v>
       </c>
       <c r="I28" s="57" t="s">
@@ -69730,28 +69734,28 @@
       </c>
     </row>
     <row r="29" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="54" t="s">
         <v>1241</v>
       </c>
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="59" t="s">
+      <c r="C29" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="60" t="s">
-        <v>1238</v>
-      </c>
-      <c r="E29" s="60" t="s">
-        <v>971</v>
-      </c>
-      <c r="F29" s="61" t="s">
+      <c r="D29" s="55" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E29" s="55" t="s">
+        <v>859</v>
+      </c>
+      <c r="F29" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="G29" s="61" t="s">
+      <c r="G29" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="H29" s="61" t="s">
+      <c r="H29" s="56" t="s">
         <v>94</v>
       </c>
       <c r="I29" s="57" t="s">
@@ -69760,7 +69764,7 @@
     </row>
     <row r="30" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="54" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="B30" s="55" t="s">
         <v>107</v>
@@ -69769,18 +69773,18 @@
         <v>108</v>
       </c>
       <c r="D30" s="55" t="s">
-        <v>1238</v>
+        <v>1250</v>
       </c>
       <c r="E30" s="55" t="s">
-        <v>977</v>
-      </c>
-      <c r="F30" s="58" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F30" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="G30" s="58" t="s">
+      <c r="G30" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="H30" s="58" t="s">
+      <c r="H30" s="56" t="s">
         <v>94</v>
       </c>
       <c r="I30" s="57" t="s">
@@ -69789,7 +69793,7 @@
     </row>
     <row r="31" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="54" t="s">
-        <v>1241</v>
+        <v>1251</v>
       </c>
       <c r="B31" s="55" t="s">
         <v>107</v>
@@ -69798,200 +69802,26 @@
         <v>108</v>
       </c>
       <c r="D31" s="55" t="s">
-        <v>1238</v>
+        <v>1250</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>980</v>
-      </c>
-      <c r="F31" s="58" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F31" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="G31" s="58" t="s">
+      <c r="G31" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="H31" s="58" t="s">
+      <c r="H31" s="56" t="s">
         <v>94</v>
       </c>
       <c r="I31" s="57" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="54" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B32" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="54" t="s">
-        <v>1242</v>
-      </c>
-      <c r="D32" s="55" t="s">
-        <v>1238</v>
-      </c>
-      <c r="E32" s="55" t="s">
-        <v>986</v>
-      </c>
-      <c r="F32" s="58" t="s">
-        <v>1243</v>
-      </c>
-      <c r="G32" s="58" t="s">
-        <v>251</v>
-      </c>
-      <c r="H32" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="I32" s="57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="54" t="s">
-        <v>1236</v>
-      </c>
-      <c r="B33" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="55" t="s">
-        <v>1238</v>
-      </c>
-      <c r="E33" s="55" t="s">
-        <v>456</v>
-      </c>
-      <c r="F33" s="58" t="s">
-        <v>250</v>
-      </c>
-      <c r="G33" s="58" t="s">
-        <v>251</v>
-      </c>
-      <c r="H33" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="I33" s="57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="54" t="s">
-        <v>1237</v>
-      </c>
-      <c r="B34" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="55" t="s">
-        <v>1249</v>
-      </c>
-      <c r="E34" s="55" t="s">
-        <v>855</v>
-      </c>
-      <c r="F34" s="56" t="s">
-        <v>250</v>
-      </c>
-      <c r="G34" s="56" t="s">
-        <v>251</v>
-      </c>
-      <c r="H34" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="I34" s="57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="54" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B35" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="55" t="s">
-        <v>1249</v>
-      </c>
-      <c r="E35" s="55" t="s">
-        <v>859</v>
-      </c>
-      <c r="F35" s="56" t="s">
-        <v>250</v>
-      </c>
-      <c r="G35" s="56" t="s">
-        <v>251</v>
-      </c>
-      <c r="H35" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="I35" s="57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="54" t="s">
-        <v>1237</v>
-      </c>
-      <c r="B36" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="55" t="s">
-        <v>1250</v>
-      </c>
-      <c r="E36" s="55" t="s">
-        <v>1146</v>
-      </c>
-      <c r="F36" s="56" t="s">
-        <v>250</v>
-      </c>
-      <c r="G36" s="56" t="s">
-        <v>251</v>
-      </c>
-      <c r="H36" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="I36" s="57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="54" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B37" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="55" t="s">
-        <v>1250</v>
-      </c>
-      <c r="E37" s="55" t="s">
-        <v>1150</v>
-      </c>
-      <c r="F37" s="56" t="s">
-        <v>250</v>
-      </c>
-      <c r="G37" s="56" t="s">
-        <v>251</v>
-      </c>
-      <c r="H37" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="I37" s="57" t="s">
-        <v>94</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I37"/>
+  <autoFilter ref="A1:I31"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
COBieLiteUK enumerations enhancements to keep it working with free spreadsheet data.
</commit_message>
<xml_diff>
--- a/Tests/TestFiles/2012-03-23-Duplex-Design.xlsx
+++ b/Tests/TestFiles/2012-03-23-Duplex-Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="252" yWindow="648" windowWidth="9756" windowHeight="9360" tabRatio="804" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="252" yWindow="648" windowWidth="9756" windowHeight="9360" tabRatio="804" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12747" uniqueCount="6703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12747" uniqueCount="6704">
   <si>
     <t>Title</t>
   </si>
@@ -20231,6 +20231,9 @@
   </si>
   <si>
     <t>Shower Stall-1, Sink Type A-1, Sink Type B-1, Sink Type C-1, Sink Type C-2, Toilet-1, Toilet-2</t>
+  </si>
+  <si>
+    <t>square meters</t>
   </si>
 </sst>
 </file>
@@ -51151,11 +51154,11 @@
   </sheetPr>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -51273,8 +51276,8 @@
       <c r="G2" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="H2" s="26" t="s">
-        <v>146</v>
+      <c r="H2" s="91" t="s">
+        <v>6703</v>
       </c>
       <c r="I2" s="26" t="s">
         <v>147</v>
@@ -68901,7 +68904,7 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>